<commit_message>
Initial Commit for Verification of Test cases
</commit_message>
<xml_diff>
--- a/Test_API.xlsx
+++ b/Test_API.xlsx
@@ -52,102 +52,111 @@
     <x:t>TestScenario_1.TestCase_1</x:t>
   </x:si>
   <x:si>
+    <x:t>GET Request</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Validate if the request type selected from the dropdown is GET</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User should be able to validate the request type is GET</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Validate in the API URL text box, a valid "ENDPOINT" is input as a URL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User should be able to validate the ENDPOINT's URL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Navigate to the Authorization tab</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User should be navigated to the Authorization Tab</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Input the Username and Password, if necessary</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User should be able to input the Username and Password</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Navigate to the Header tab</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User should be navigated to the Header Tab</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Input the data, if necessary</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User should be able to input the data for the fields</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Navigate to the Body tab</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User should be navigated to the Body tab</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Navigate to the Test tab</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User should be navigated to the Test tab</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Select the appropriate test(s) by selecting the corresponding CheckBox</x:t>
+  </x:si>
+  <x:si>
+    <x:t>User should be able to select appropriate Test(s) by selecting the CheckBoxes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Step 11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Click on Save to save the configuration</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Configuration Saved success message should be displayed</x:t>
+  </x:si>
+  <x:si>
     <x:t>POST Request</x:t>
   </x:si>
   <x:si>
-    <x:t>Step 1</x:t>
-  </x:si>
-  <x:si>
     <x:t>Validate if the request type selected from the dropdown is POST</x:t>
   </x:si>
   <x:si>
     <x:t>User should be able to validate the request type is POST</x:t>
   </x:si>
   <x:si>
-    <x:t>Step 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Validate in the API URL text box, a valid "ENDPOINT" is input as a URL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User should be able to validate the ENDPOINT's URL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Step 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Navigate to the Authorization tab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User should be navigated to the Authorization Tab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Step 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Input the Username and Password, if necessary</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User should be able to input the Username and Password</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Step 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Navigate to the Header tab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User should be navigated to the Header Tab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Step 6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Input the data, if necessary</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User should be able to input the data for the fields</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Step 7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Navigate to the Body tab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User should be navigated to the Body tab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Step 8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Step 9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Navigate to the Test tab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User should be navigated to the Test tab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Step 10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Select the appropriate test(s) by selecting the corresponding CheckBox</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User should be able to select appropriate Test(s) by selecting the CheckBoxes</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Step 11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Click on Save to save the configuration</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Configuration Saved success message should be displayed</x:t>
-  </x:si>
-  <x:si>
     <x:t>PUT Request</x:t>
   </x:si>
   <x:si>
@@ -164,15 +173,6 @@
   </x:si>
   <x:si>
     <x:t>User should be able to validate the request type is DELETE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GET Request</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Validate if the request type selected from the dropdown is GET</x:t>
-  </x:si>
-  <x:si>
-    <x:t>User should be able to validate the request type is GET</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>